<commit_message>
Material switched to plants
All looking good, Blessings would be next
</commit_message>
<xml_diff>
--- a/Ressourcen/Docs/Plants Doc.xlsx
+++ b/Ressourcen/Docs/Plants Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Repositories\Dreamers-Garden_Game\Ressourcen\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7943E1-3B42-4A8A-AF00-7A08607EDA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01775C1-4C67-4CDB-8CA5-0583ADE39201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{CFC539C6-04FB-435C-B762-9D2E1EF00861}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="19200" windowHeight="9970" xr2:uid="{CFC539C6-04FB-435C-B762-9D2E1EF00861}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="206">
   <si>
     <t xml:space="preserve">Destroy a card </t>
   </si>
@@ -651,6 +651,9 @@
   </si>
   <si>
     <t>Weed</t>
+  </si>
+  <si>
+    <t>It needs a while, but will deliver a lot of deadwood once grown.</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1112,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1221,7 +1224,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>111</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1249,11 +1252,11 @@
         <v>50</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>99</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1301,7 +1304,7 @@
         <v>81</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>83</v>
+        <v>205</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>6</v>

</xml_diff>